<commit_message>
salary prediction UI  🐼
</commit_message>
<xml_diff>
--- a/project_data/generated_data/users.xlsx
+++ b/project_data/generated_data/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -751,6 +751,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Diya</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>